<commit_message>
Se refactoriza la tarea SolicitarEprepago
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/e-prepago/eprepago.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/e-prepago/eprepago.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\appOPS\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\e-prepago\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9541C6C-9E28-4504-B8BD-F4F6946C6605}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0883D23-8ACC-4011-9FFE-312A0C94261E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -143,10 +143,10 @@
     <t>Consultas</t>
   </si>
   <si>
-    <t>sineprepago1</t>
-  </si>
-  <si>
     <t>autotest11</t>
+  </si>
+  <si>
+    <t>userunico01</t>
   </si>
 </sst>
 </file>
@@ -534,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
@@ -596,7 +596,7 @@
         <v>13</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>14</v>
@@ -637,7 +637,7 @@
         <v>13</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Se agrega correo en el archivo datadriven, inscripcion de e-prepago
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/e-prepago/eprepago.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/e-prepago/eprepago.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\appOPS\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\e-prepago\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0883D23-8ACC-4011-9FFE-312A0C94261E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7865A0FB-9070-4C4A-8DCB-AC15885EA413}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
   <si>
     <t>ID</t>
   </si>
@@ -147,13 +147,19 @@
   </si>
   <si>
     <t>userunico01</t>
+  </si>
+  <si>
+    <t>correoUsuario</t>
+  </si>
+  <si>
+    <t>jruav@devco.com.co</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -191,6 +197,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -218,7 +232,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -241,12 +255,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -256,8 +282,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
@@ -532,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
@@ -544,7 +572,7 @@
     <col min="13" max="13" width="21.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -584,8 +612,11 @@
       <c r="M1" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
@@ -625,8 +656,11 @@
       <c r="M2" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="N2" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="6" t="s">
         <v>23</v>
       </c>
@@ -667,12 +701,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:14">
       <c r="M7" s="8"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="N2" r:id="rId1" xr:uid="{60AD2053-1B80-4BF7-BE27-49F67FC03F39}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Se refactoriza la tarea SolicitudEprepago, se refactoriza el feature solicitar_eprepago
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/e-prepago/eprepago.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/e-prepago/eprepago.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\appOPS\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\e-prepago\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7865A0FB-9070-4C4A-8DCB-AC15885EA413}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E378DA44-6D96-4E69-BC2A-253BFDF917BE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
   <si>
     <t>ID</t>
   </si>
@@ -149,10 +149,19 @@
     <t>userunico01</t>
   </si>
   <si>
-    <t>correoUsuario</t>
-  </si>
-  <si>
-    <t>jruav@devco.com.co</t>
+    <t>jrua@todo1.net</t>
+  </si>
+  <si>
+    <t>tipoCorreo</t>
+  </si>
+  <si>
+    <t>Laboral</t>
+  </si>
+  <si>
+    <t>correo</t>
+  </si>
+  <si>
+    <t>numeroCelular</t>
   </si>
 </sst>
 </file>
@@ -272,7 +281,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -283,6 +292,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
@@ -560,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
@@ -572,7 +582,7 @@
     <col min="13" max="13" width="21.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -613,10 +623,16 @@
         <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
+        <v>45</v>
+      </c>
+      <c r="O1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
@@ -657,10 +673,16 @@
         <v>22</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
+        <v>42</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="P2">
+        <v>3146834995</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3" s="6" t="s">
         <v>23</v>
       </c>
@@ -701,7 +723,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:16">
       <c r="M7" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactorización escenario Solicitud de un cliente que ya tiene tarjeta eprepago, se valida la question y se cambian mapeos
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/e-prepago/eprepago.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/e-prepago/eprepago.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\appOPS\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\e-prepago\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E378DA44-6D96-4E69-BC2A-253BFDF917BE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85CFAEDB-6F23-4B5A-BFD0-99C9B4667865}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
   <si>
     <t>ID</t>
   </si>
@@ -141,9 +141,6 @@
   </si>
   <si>
     <t>Consultas</t>
-  </si>
-  <si>
-    <t>autotest11</t>
   </si>
   <si>
     <t>userunico01</t>
@@ -281,7 +278,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -293,6 +290,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
@@ -572,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
@@ -623,13 +622,13 @@
         <v>12</v>
       </c>
       <c r="N1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P1" t="s">
         <v>45</v>
-      </c>
-      <c r="O1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -643,7 +642,7 @@
         <v>13</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>14</v>
@@ -673,10 +672,10 @@
         <v>22</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P2">
         <v>3146834995</v>
@@ -687,7 +686,7 @@
         <v>23</v>
       </c>
       <c r="B3" s="3">
-        <v>48646663</v>
+        <v>928155907</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>13</v>
@@ -721,6 +720,15 @@
       </c>
       <c r="M3" s="3" t="s">
         <v>22</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="O3" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="P3">
+        <v>3146834995</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -729,9 +737,10 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="N2" r:id="rId1" xr:uid="{60AD2053-1B80-4BF7-BE27-49F67FC03F39}"/>
+    <hyperlink ref="N3" r:id="rId2" xr:uid="{AE68C3DB-30C6-4860-B024-7970D79080F9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Refactorización de la tarea SolicitarEprepago
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/e-prepago/eprepago.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/e-prepago/eprepago.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\appOPS\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\e-prepago\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85CFAEDB-6F23-4B5A-BFD0-99C9B4667865}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F975F76-F189-4FD5-AA7B-6B8A36ED45DC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
   <si>
     <t>ID</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>numeroCelular</t>
+  </si>
+  <si>
+    <t>autotest27</t>
   </si>
 </sst>
 </file>
@@ -278,7 +281,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -292,6 +295,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
@@ -571,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
@@ -635,14 +641,14 @@
       <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="3">
-        <v>928155907</v>
+      <c r="B2" s="13">
+        <v>93221452</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Se refactoriza la tarea solicitarEprepago, se refactorizan los mapeos de la clase SolicitudEprepagoLocator, se agrega el xpath Solicitar a la clase GeneralLocator, se refactoriza el archivo solicitar_e_prepago
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/e-prepago/eprepago.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/e-prepago/eprepago.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\appOPS\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\e-prepago\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CEFABA5-8BF8-485E-B975-834C1124E093}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2DD8C7-4FDF-42FF-8E39-F8DE5AFCFCCC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
   <si>
     <t>ID</t>
   </si>
@@ -144,21 +144,6 @@
   </si>
   <si>
     <t>userunico01</t>
-  </si>
-  <si>
-    <t>jrua@todo1.net</t>
-  </si>
-  <si>
-    <t>tipoCorreo</t>
-  </si>
-  <si>
-    <t>Laboral</t>
-  </si>
-  <si>
-    <t>correo</t>
-  </si>
-  <si>
-    <t>numeroCelular</t>
   </si>
   <si>
     <t>autotest27</t>
@@ -281,7 +266,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -295,6 +280,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
@@ -572,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
@@ -584,7 +572,7 @@
     <col min="13" max="13" width="21.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -624,28 +612,19 @@
       <c r="M1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
-        <v>44</v>
-      </c>
-      <c r="O1" t="s">
-        <v>42</v>
-      </c>
-      <c r="P1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="13">
         <v>93221452</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>14</v>
@@ -674,17 +653,10 @@
       <c r="M2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="O2" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="P2">
-        <v>3146834995</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="N2" s="9"/>
+      <c r="O2" s="10"/>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="6" t="s">
         <v>23</v>
       </c>
@@ -724,26 +696,15 @@
       <c r="M3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="O3" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="P3">
-        <v>3146834995</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="N3" s="11"/>
+      <c r="O3" s="12"/>
+    </row>
+    <row r="7" spans="1:15">
       <c r="M7" s="8"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="N2" r:id="rId1" xr:uid="{60AD2053-1B80-4BF7-BE27-49F67FC03F39}"/>
-    <hyperlink ref="N3" r:id="rId2" xr:uid="{AE68C3DB-30C6-4860-B024-7970D79080F9}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Refactorización de la clase SolicitarEprepago, se refactoriza el archivo solicitar_e_prepago, se configura la data en el excel eprepago
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/e-prepago/eprepago.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/e-prepago/eprepago.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\appOPS\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\e-prepago\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F975F76-F189-4FD5-AA7B-6B8A36ED45DC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F3F5EB-97BF-4E8E-AC46-CB0030C77459}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
   <si>
     <t>ID</t>
   </si>
@@ -141,24 +141,6 @@
   </si>
   <si>
     <t>Consultas</t>
-  </si>
-  <si>
-    <t>userunico01</t>
-  </si>
-  <si>
-    <t>jrua@todo1.net</t>
-  </si>
-  <si>
-    <t>tipoCorreo</t>
-  </si>
-  <si>
-    <t>Laboral</t>
-  </si>
-  <si>
-    <t>correo</t>
-  </si>
-  <si>
-    <t>numeroCelular</t>
   </si>
   <si>
     <t>autotest27</t>
@@ -575,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
@@ -587,7 +569,7 @@
     <col min="13" max="13" width="21.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -627,17 +609,8 @@
       <c r="M1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
-        <v>44</v>
-      </c>
-      <c r="O1" t="s">
-        <v>42</v>
-      </c>
-      <c r="P1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
@@ -648,7 +621,7 @@
         <v>13</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>14</v>
@@ -677,22 +650,15 @@
       <c r="M2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="O2" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="P2">
-        <v>3146834995</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="N2" s="9"/>
+      <c r="O2" s="10"/>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="3">
-        <v>928155907</v>
+      <c r="B3" s="13">
+        <v>93221452</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>13</v>
@@ -727,26 +693,15 @@
       <c r="M3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="O3" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="P3">
-        <v>3146834995</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="N3" s="11"/>
+      <c r="O3" s="12"/>
+    </row>
+    <row r="7" spans="1:15">
       <c r="M7" s="8"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="N2" r:id="rId1" xr:uid="{60AD2053-1B80-4BF7-BE27-49F67FC03F39}"/>
-    <hyperlink ref="N3" r:id="rId2" xr:uid="{AE68C3DB-30C6-4860-B024-7970D79080F9}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>